<commit_message>
As a lead I have created Hybrid TestNG Framework.Login and Register.
</commit_message>
<xml_diff>
--- a/src/main/java/com/tutorialsninja/qa/testData/TutorialsNinjaTestData.xlsx
+++ b/src/main/java/com/tutorialsninja/qa/testData/TutorialsNinjaTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHEERENDRA\eclipse-workspace\TutorialsNinjaProject\src\main\java\com\tutorialsninja\qa\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHEERENDRA\git\DKRepo\src\main\java\com\tutorialsninja\qa\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B2353D-7964-4A5F-B4C2-230F74DC2BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF99AA46-6C8E-473B-8BE7-E311979EF663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Email</t>
   </si>
@@ -40,13 +40,16 @@
   </si>
   <si>
     <t>dheeruvish1610@gmail.com</t>
+  </si>
+  <si>
+    <t>dheeruvish1611@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +61,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,11 +428,21 @@
         <v>987374623</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>988657464</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{39F7E305-7DD8-4042-81C7-7C907DCA22BC}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{66BCBEA2-E708-4BDF-943D-A88963CF7805}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{8912AADC-4B8B-4D75-9BB4-747BF8692B6B}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{12A191FC-55C0-4F03-B3A7-A45F62D9EF54}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>